<commit_message>
knip Arbeidsmodaliteit.adl los van Dagverantwoordingen.adl
</commit_message>
<xml_diff>
--- a/NVWA DTV/Arbeidsmodaliteiten.xlsx
+++ b/NVWA DTV/Arbeidsmodaliteiten.xlsx
@@ -8,36 +8,29 @@
   </bookViews>
   <sheets>
     <sheet name="adhoc - Roosters " sheetId="15" r:id="rId1"/>
-    <sheet name="Dagverantwoording" sheetId="2" r:id="rId2"/>
-    <sheet name="Modaliteit" sheetId="3" r:id="rId3"/>
-    <sheet name="Personeelsnummer" sheetId="4" r:id="rId4"/>
-    <sheet name="Tijdvak" sheetId="5" r:id="rId5"/>
-    <sheet name="arbeidsmod" sheetId="7" r:id="rId6"/>
-    <sheet name="arbeidsmodaliteitIngangsdatum" sheetId="8" r:id="rId7"/>
-    <sheet name="binnenTijdvak" sheetId="9" r:id="rId8"/>
-    <sheet name="date" sheetId="10" r:id="rId9"/>
-    <sheet name="geqDatum" sheetId="11" r:id="rId10"/>
-    <sheet name="geqTijdstip" sheetId="12" r:id="rId11"/>
-    <sheet name="gtDatum" sheetId="13" r:id="rId12"/>
-    <sheet name="overlap" sheetId="14" r:id="rId13"/>
+    <sheet name="Modaliteit" sheetId="3" r:id="rId2"/>
+    <sheet name="Personeelsnummer" sheetId="4" r:id="rId3"/>
+    <sheet name="Tijdvak" sheetId="5" r:id="rId4"/>
+    <sheet name="arbeidsmod" sheetId="7" r:id="rId5"/>
+    <sheet name="arbeidsmodaliteitIngangsdatum" sheetId="8" r:id="rId6"/>
+    <sheet name="binnenTijdvak" sheetId="9" r:id="rId7"/>
+    <sheet name="date" sheetId="10" r:id="rId8"/>
+    <sheet name="geqDatum" sheetId="11" r:id="rId9"/>
+    <sheet name="geqTijdstip" sheetId="12" r:id="rId10"/>
+    <sheet name="gtDatum" sheetId="13" r:id="rId11"/>
+    <sheet name="overlap" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="46">
   <si>
     <t>Aantaldagen</t>
   </si>
   <si>
     <t>Arbeidsmodaliteit</t>
-  </si>
-  <si>
-    <t>Dagsoort</t>
-  </si>
-  <si>
-    <t>Dagverantwoording</t>
   </si>
   <si>
     <t>DateTime</t>
@@ -68,9 +61,6 @@
   </si>
   <si>
     <t>[Arbeidsmodaliteit]</t>
-  </si>
-  <si>
-    <t>[Dagverantwoording]</t>
   </si>
   <si>
     <t>[DateTime]</t>
@@ -118,13 +108,7 @@
     <t>dag_Tijdverantwoording</t>
   </si>
   <si>
-    <t>dagsoort</t>
-  </si>
-  <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>datum</t>
   </si>
   <si>
     <t>eind</t>
@@ -568,37 +552,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -638,7 +622,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -798,7 +782,7 @@
         <v>9</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -878,7 +862,7 @@
         <v>4</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -886,7 +870,7 @@
         <v>20046659</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C16" s="8">
         <v>9</v>
@@ -901,7 +885,7 @@
         <v>9</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H16" s="8">
         <v>9</v>
@@ -1033,7 +1017,7 @@
         <v>9</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="8" customFormat="1">
@@ -1133,7 +1117,7 @@
         <v>9</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="8" customFormat="1">
@@ -1213,7 +1197,7 @@
         <v>9</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="8" customFormat="1">
@@ -1253,7 +1237,7 @@
         <v>9</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G33" s="8">
         <v>9</v>
@@ -1268,7 +1252,7 @@
         <v>9</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -1508,7 +1492,7 @@
         <v>8</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -1622,7 +1606,7 @@
         <v>8</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E51" s="8">
         <v>8</v>
@@ -1668,7 +1652,7 @@
         <v>9</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G53" s="8">
         <v>9</v>
@@ -1717,7 +1701,7 @@
         <v>9</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E55" s="8">
         <v>9</v>
@@ -1742,18 +1726,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1771,18 +1755,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1800,47 +1784,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1850,52 +1805,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C999"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1907,24 +1820,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -15890,7 +15803,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B500"/>
   <sheetViews>
@@ -15907,15 +15820,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>1</v>
@@ -20907,7 +20820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M2"/>
   <sheetViews>
@@ -20932,66 +20845,66 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
         <v>26</v>
-      </c>
-      <c r="H1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
       <c r="I2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -20999,7 +20912,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W500"/>
   <sheetViews>
@@ -21020,37 +20933,37 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -21090,40 +21003,40 @@
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="3" customFormat="1">
@@ -21135,34 +21048,34 @@
         <v>[Modaliteit8]</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -44166,7 +44079,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B500"/>
   <sheetViews>
@@ -44182,10 +44095,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -44193,7 +44106,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -48676,6 +48589,35 @@
       </c>
       <c r="B500" s="9">
         <v>42005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -48693,7 +48635,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>27</v>
@@ -48701,10 +48643,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -48722,18 +48664,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Referentielijsten werkt samen met Arbeidsmodaliteiten.
Voor het inladen van gegevens over Arbeidsmodaliteiten moet het bestand Arbeidsmodaliteiten.xlsx via de user-interface worden ingeladen. Via het include mechaniek werkt het (nog) niet.
</commit_message>
<xml_diff>
--- a/NVWA DTV/Arbeidsmodaliteiten.xlsx
+++ b/NVWA DTV/Arbeidsmodaliteiten.xlsx
@@ -4,24 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="10860" windowHeight="8532" tabRatio="764" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="10860" windowHeight="8532" tabRatio="764"/>
   </bookViews>
   <sheets>
     <sheet name="voor runtime loader" sheetId="3" r:id="rId1"/>
-    <sheet name="adhoc - Roosters " sheetId="15" r:id="rId2"/>
-    <sheet name="Arbeidsmodaliteiten" sheetId="16" r:id="rId3"/>
-    <sheet name="Modaliteit" sheetId="17" r:id="rId4"/>
-    <sheet name="Variables" sheetId="18" r:id="rId5"/>
+    <sheet name="voor debugging" sheetId="19" r:id="rId2"/>
+    <sheet name="adhoc - Roosters " sheetId="15" r:id="rId3"/>
+    <sheet name="Arbeidsmodaliteiten" sheetId="16" r:id="rId4"/>
+    <sheet name="Modaliteit" sheetId="17" r:id="rId5"/>
+    <sheet name="Variables" sheetId="18" r:id="rId6"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-  </externalReferences>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="672">
   <si>
     <t>Arbeidsmodaliteit</t>
   </si>
@@ -2106,298 +2104,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="adhoc - Roosters "/>
-      <sheetName val="Arbeidsmodaliteiten"/>
-      <sheetName val="Modaliteit"/>
-      <sheetName val="Variables"/>
-      <sheetName val="Mutation"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="B3">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="B26">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="B27">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="B29">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="B31">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="B32">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="B33">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="B34">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="B35">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="B36">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="B37">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="B38">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="B39">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="B40">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="B41">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="B42">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="B43">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="B44">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="B45">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="B46">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="B47">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="B48">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="B49">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="B50">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="B51">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="B52">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="B53">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="B54">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="B55">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="B56">
-            <v>42005</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2687,8 +2393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E599"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -12533,6 +12239,139 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L501"/>
   <sheetViews>
@@ -16127,7 +15966,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D56"/>
   <sheetViews>
@@ -16178,7 +16017,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D3" s="8">
-        <f>'[1]adhoc - Roosters '!B3</f>
+        <f>'adhoc - Roosters '!B3</f>
         <v>42005</v>
       </c>
     </row>
@@ -16196,7 +16035,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D4" s="8">
-        <f>'[1]adhoc - Roosters '!B4</f>
+        <f>'adhoc - Roosters '!B4</f>
         <v>42005</v>
       </c>
     </row>
@@ -16214,7 +16053,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D5" s="8">
-        <f>'[1]adhoc - Roosters '!B5</f>
+        <f>'adhoc - Roosters '!B5</f>
         <v>42005</v>
       </c>
     </row>
@@ -16232,7 +16071,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D6" s="8">
-        <f>'[1]adhoc - Roosters '!B6</f>
+        <f>'adhoc - Roosters '!B6</f>
         <v>42005</v>
       </c>
     </row>
@@ -16250,7 +16089,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D7" s="8">
-        <f>'[1]adhoc - Roosters '!B7</f>
+        <f>'adhoc - Roosters '!B7</f>
         <v>42005</v>
       </c>
     </row>
@@ -16268,7 +16107,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D8" s="8">
-        <f>'[1]adhoc - Roosters '!B8</f>
+        <f>'adhoc - Roosters '!B8</f>
         <v>42005</v>
       </c>
     </row>
@@ -16286,7 +16125,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D9" s="8">
-        <f>'[1]adhoc - Roosters '!B9</f>
+        <f>'adhoc - Roosters '!B9</f>
         <v>42005</v>
       </c>
     </row>
@@ -16304,7 +16143,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D10" s="8">
-        <f>'[1]adhoc - Roosters '!B10</f>
+        <f>'adhoc - Roosters '!B10</f>
         <v>42005</v>
       </c>
     </row>
@@ -16322,7 +16161,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D11" s="8">
-        <f>'[1]adhoc - Roosters '!B11</f>
+        <f>'adhoc - Roosters '!B11</f>
         <v>42005</v>
       </c>
     </row>
@@ -16340,7 +16179,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D12" s="8">
-        <f>'[1]adhoc - Roosters '!B12</f>
+        <f>'adhoc - Roosters '!B12</f>
         <v>42005</v>
       </c>
     </row>
@@ -16358,7 +16197,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D13" s="8">
-        <f>'[1]adhoc - Roosters '!B13</f>
+        <f>'adhoc - Roosters '!B13</f>
         <v>42005</v>
       </c>
     </row>
@@ -16376,7 +16215,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D14" s="8">
-        <f>'[1]adhoc - Roosters '!B14</f>
+        <f>'adhoc - Roosters '!B14</f>
         <v>42005</v>
       </c>
     </row>
@@ -16394,7 +16233,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D15" s="8">
-        <f>'[1]adhoc - Roosters '!B15</f>
+        <f>'adhoc - Roosters '!B15</f>
         <v>42005</v>
       </c>
     </row>
@@ -16412,7 +16251,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D16" s="8">
-        <f>'[1]adhoc - Roosters '!B16</f>
+        <f>'adhoc - Roosters '!B16</f>
         <v>42005</v>
       </c>
     </row>
@@ -16430,7 +16269,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D17" s="8">
-        <f>'[1]adhoc - Roosters '!B17</f>
+        <f>'adhoc - Roosters '!B17</f>
         <v>42005</v>
       </c>
     </row>
@@ -16448,7 +16287,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D18" s="8">
-        <f>'[1]adhoc - Roosters '!B18</f>
+        <f>'adhoc - Roosters '!B18</f>
         <v>42005</v>
       </c>
     </row>
@@ -16466,7 +16305,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D19" s="8">
-        <f>'[1]adhoc - Roosters '!B19</f>
+        <f>'adhoc - Roosters '!B19</f>
         <v>42005</v>
       </c>
     </row>
@@ -16484,7 +16323,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D20" s="8">
-        <f>'[1]adhoc - Roosters '!B20</f>
+        <f>'adhoc - Roosters '!B20</f>
         <v>42005</v>
       </c>
     </row>
@@ -16502,7 +16341,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D21" s="8">
-        <f>'[1]adhoc - Roosters '!B21</f>
+        <f>'adhoc - Roosters '!B21</f>
         <v>42005</v>
       </c>
     </row>
@@ -16520,7 +16359,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D22" s="8">
-        <f>'[1]adhoc - Roosters '!B22</f>
+        <f>'adhoc - Roosters '!B22</f>
         <v>42005</v>
       </c>
     </row>
@@ -16538,7 +16377,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D23" s="8">
-        <f>'[1]adhoc - Roosters '!B23</f>
+        <f>'adhoc - Roosters '!B23</f>
         <v>42005</v>
       </c>
     </row>
@@ -16556,7 +16395,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D24" s="8">
-        <f>'[1]adhoc - Roosters '!B24</f>
+        <f>'adhoc - Roosters '!B24</f>
         <v>42005</v>
       </c>
     </row>
@@ -16574,7 +16413,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D25" s="8">
-        <f>'[1]adhoc - Roosters '!B25</f>
+        <f>'adhoc - Roosters '!B25</f>
         <v>42005</v>
       </c>
     </row>
@@ -16592,7 +16431,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D26" s="8">
-        <f>'[1]adhoc - Roosters '!B26</f>
+        <f>'adhoc - Roosters '!B26</f>
         <v>42005</v>
       </c>
     </row>
@@ -16610,7 +16449,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D27" s="8">
-        <f>'[1]adhoc - Roosters '!B27</f>
+        <f>'adhoc - Roosters '!B27</f>
         <v>42005</v>
       </c>
     </row>
@@ -16628,7 +16467,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D28" s="8">
-        <f>'[1]adhoc - Roosters '!B28</f>
+        <f>'adhoc - Roosters '!B28</f>
         <v>42005</v>
       </c>
     </row>
@@ -16646,7 +16485,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D29" s="8">
-        <f>'[1]adhoc - Roosters '!B29</f>
+        <f>'adhoc - Roosters '!B29</f>
         <v>42005</v>
       </c>
     </row>
@@ -16664,7 +16503,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D30" s="8">
-        <f>'[1]adhoc - Roosters '!B30</f>
+        <f>'adhoc - Roosters '!B30</f>
         <v>42005</v>
       </c>
     </row>
@@ -16682,7 +16521,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D31" s="8">
-        <f>'[1]adhoc - Roosters '!B31</f>
+        <f>'adhoc - Roosters '!B31</f>
         <v>42005</v>
       </c>
     </row>
@@ -16700,7 +16539,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D32" s="8">
-        <f>'[1]adhoc - Roosters '!B32</f>
+        <f>'adhoc - Roosters '!B32</f>
         <v>42005</v>
       </c>
     </row>
@@ -16718,7 +16557,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D33" s="8">
-        <f>'[1]adhoc - Roosters '!B33</f>
+        <f>'adhoc - Roosters '!B33</f>
         <v>42005</v>
       </c>
     </row>
@@ -16736,7 +16575,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D34" s="8">
-        <f>'[1]adhoc - Roosters '!B34</f>
+        <f>'adhoc - Roosters '!B34</f>
         <v>42005</v>
       </c>
     </row>
@@ -16750,11 +16589,11 @@
         <v>20047188</v>
       </c>
       <c r="C35" s="7" t="str">
-        <f t="shared" ref="C35:C66" si="1">TEXT(D35,"d-m-jjjj")</f>
+        <f t="shared" ref="C35:C56" si="1">TEXT(D35,"d-m-jjjj")</f>
         <v>1-1-2015</v>
       </c>
       <c r="D35" s="8">
-        <f>'[1]adhoc - Roosters '!B35</f>
+        <f>'adhoc - Roosters '!B35</f>
         <v>42005</v>
       </c>
     </row>
@@ -16772,7 +16611,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D36" s="8">
-        <f>'[1]adhoc - Roosters '!B36</f>
+        <f>'adhoc - Roosters '!B36</f>
         <v>42005</v>
       </c>
     </row>
@@ -16790,7 +16629,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D37" s="8">
-        <f>'[1]adhoc - Roosters '!B37</f>
+        <f>'adhoc - Roosters '!B37</f>
         <v>42005</v>
       </c>
     </row>
@@ -16808,7 +16647,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D38" s="8">
-        <f>'[1]adhoc - Roosters '!B38</f>
+        <f>'adhoc - Roosters '!B38</f>
         <v>42005</v>
       </c>
     </row>
@@ -16826,7 +16665,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D39" s="8">
-        <f>'[1]adhoc - Roosters '!B39</f>
+        <f>'adhoc - Roosters '!B39</f>
         <v>42005</v>
       </c>
     </row>
@@ -16844,7 +16683,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D40" s="8">
-        <f>'[1]adhoc - Roosters '!B40</f>
+        <f>'adhoc - Roosters '!B40</f>
         <v>42005</v>
       </c>
     </row>
@@ -16862,7 +16701,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D41" s="8">
-        <f>'[1]adhoc - Roosters '!B41</f>
+        <f>'adhoc - Roosters '!B41</f>
         <v>42005</v>
       </c>
     </row>
@@ -16880,7 +16719,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D42" s="8">
-        <f>'[1]adhoc - Roosters '!B42</f>
+        <f>'adhoc - Roosters '!B42</f>
         <v>42005</v>
       </c>
     </row>
@@ -16898,7 +16737,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D43" s="8">
-        <f>'[1]adhoc - Roosters '!B43</f>
+        <f>'adhoc - Roosters '!B43</f>
         <v>42005</v>
       </c>
     </row>
@@ -16916,7 +16755,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D44" s="8">
-        <f>'[1]adhoc - Roosters '!B44</f>
+        <f>'adhoc - Roosters '!B44</f>
         <v>42005</v>
       </c>
     </row>
@@ -16934,7 +16773,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D45" s="8">
-        <f>'[1]adhoc - Roosters '!B45</f>
+        <f>'adhoc - Roosters '!B45</f>
         <v>42005</v>
       </c>
     </row>
@@ -16952,7 +16791,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D46" s="8">
-        <f>'[1]adhoc - Roosters '!B46</f>
+        <f>'adhoc - Roosters '!B46</f>
         <v>42005</v>
       </c>
     </row>
@@ -16970,7 +16809,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D47" s="8">
-        <f>'[1]adhoc - Roosters '!B47</f>
+        <f>'adhoc - Roosters '!B47</f>
         <v>42005</v>
       </c>
     </row>
@@ -16988,7 +16827,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D48" s="8">
-        <f>'[1]adhoc - Roosters '!B48</f>
+        <f>'adhoc - Roosters '!B48</f>
         <v>42005</v>
       </c>
     </row>
@@ -17006,7 +16845,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D49" s="8">
-        <f>'[1]adhoc - Roosters '!B49</f>
+        <f>'adhoc - Roosters '!B49</f>
         <v>42005</v>
       </c>
     </row>
@@ -17024,7 +16863,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D50" s="8">
-        <f>'[1]adhoc - Roosters '!B50</f>
+        <f>'adhoc - Roosters '!B50</f>
         <v>42005</v>
       </c>
     </row>
@@ -17042,7 +16881,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D51" s="8">
-        <f>'[1]adhoc - Roosters '!B51</f>
+        <f>'adhoc - Roosters '!B51</f>
         <v>42005</v>
       </c>
     </row>
@@ -17060,7 +16899,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D52" s="8">
-        <f>'[1]adhoc - Roosters '!B52</f>
+        <f>'adhoc - Roosters '!B52</f>
         <v>42005</v>
       </c>
     </row>
@@ -17078,7 +16917,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D53" s="8">
-        <f>'[1]adhoc - Roosters '!B53</f>
+        <f>'adhoc - Roosters '!B53</f>
         <v>42005</v>
       </c>
     </row>
@@ -17096,7 +16935,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D54" s="8">
-        <f>'[1]adhoc - Roosters '!B54</f>
+        <f>'adhoc - Roosters '!B54</f>
         <v>42005</v>
       </c>
     </row>
@@ -17114,7 +16953,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D55" s="8">
-        <f>'[1]adhoc - Roosters '!B55</f>
+        <f>'adhoc - Roosters '!B55</f>
         <v>42005</v>
       </c>
     </row>
@@ -17132,7 +16971,7 @@
         <v>1-1-2015</v>
       </c>
       <c r="D56" s="8">
-        <f>'[1]adhoc - Roosters '!B56</f>
+        <f>'adhoc - Roosters '!B56</f>
         <v>42005</v>
       </c>
     </row>
@@ -17141,7 +16980,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H542"/>
   <sheetViews>
@@ -35557,11 +35396,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>